<commit_message>
doing lots of things
</commit_message>
<xml_diff>
--- a/1 Output/Ex 2/Ex 2 Cleaned/Full Data Ex 2.xlsx
+++ b/1 Output/Ex 2/Ex 2 Cleaned/Full Data Ex 2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nickm.000\Documents\GitHub\Trevor-Honors-Thesis\1 Output\Ex2\Ex 2 Cleaned\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nickm.000\Documents\GitHub\Trevor-Honors-Thesis\1 Output\Ex 2\Ex 2 Cleaned\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF9CDEF3-D0D4-4801-B799-AC2385C56F60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1FAFF56-9D57-4FA1-BDAD-D1D98C4F9731}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11280" xr2:uid="{DBBA9ECF-A48D-4BE5-A2D5-A05C1F36FF92}"/>
   </bookViews>
@@ -789,8 +789,8 @@
   <dimension ref="A1:S50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C53" sqref="C53"/>
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -839,50 +839,50 @@
       <c r="R1" s="2"/>
       <c r="S1" s="2"/>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="Q2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="R2" t="s">
+      <c r="R2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="S2" t="s">
+      <c r="S2" s="3" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>